<commit_message>
upgrade to the final version
</commit_message>
<xml_diff>
--- a/mapilot_compare_result.xlsx
+++ b/mapilot_compare_result.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[41.3642604, 2.1344993]</t>
+          <t>41.3642604,2.1344993</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -497,7 +497,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[41.3621909, 2.1317393]</t>
+          <t>41.3621909,2.1317393</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[41.3475633, 2.1122495999999997]</t>
+          <t>41.3475633,2.1122495999999997</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -543,7 +543,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[41.4196, 2.0017889]</t>
+          <t>41.4196,2.0017889</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[41.4195845, 2.0016996]</t>
+          <t>41.4195845,2.0016996</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -587,7 +587,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[41.4195583, 2.0015478]</t>
+          <t>41.4195583,2.0015478</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[41.4195479, 2.001486]</t>
+          <t>41.4195479,2.001486</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -631,7 +631,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[41.4195375, 2.0014317999999998]</t>
+          <t>41.4195375,2.0014317999999998</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[41.4196199, 2.0011223]</t>
+          <t>41.4196199,2.0011223</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -675,7 +675,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[41.4196762, 2.0011019]</t>
+          <t>41.4196762,2.0011019</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -697,7 +697,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[41.4197408, 2.0010784]</t>
+          <t>41.4197408,2.0010784</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -719,7 +719,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[41.4198808, 2.0010332]</t>
+          <t>41.4198808,2.0010332</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -741,7 +741,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[41.4199518, 2.0010079000000003]</t>
+          <t>41.4199518,2.0010079000000003</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[41.4200888, 2.000958]</t>
+          <t>41.4200888,2.000958</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -785,7 +785,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[41.4202254, 2.0009078]</t>
+          <t>41.4202254,2.0009078</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -807,7 +807,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[41.4202923, 2.000883]</t>
+          <t>41.4202923,2.000883</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[41.428946, 1.9954136999999998]</t>
+          <t>41.428946,1.9954136999999998</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[41.429212799999995, 1.9953535999999998]</t>
+          <t>41.429212799999995,1.9953535999999998</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -873,7 +873,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[41.429354700000005, 1.9953214000000001]</t>
+          <t>41.429354700000005,1.9953214000000001</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -895,7 +895,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[41.4294971, 1.9952883]</t>
+          <t>41.4294971,1.9952883</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -917,7 +917,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[41.429791800000004, 1.9952096]</t>
+          <t>41.429791800000004,1.9952096</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -939,7 +939,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[41.4299426, 1.9951629999999998]</t>
+          <t>41.4299426,1.9951629999999998</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -961,7 +961,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[41.4302565, 1.9950503]</t>
+          <t>41.4302565,1.9950503</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -983,7 +983,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[41.4304168, 1.9949887]</t>
+          <t>41.4304168,1.9949887</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[41.4305789, 1.9949227999999999]</t>
+          <t>41.4305789,1.9949227999999999</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[41.4307434, 1.9948542999999999]</t>
+          <t>41.4307434,1.9948542999999999</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[41.4309119, 1.9947879000000002]</t>
+          <t>41.4309119,1.9947879000000002</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[41.4429511, 1.9821202]</t>
+          <t>41.4429511,1.9821202</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[41.4431496, 1.9818878]</t>
+          <t>41.4431496,1.9818878</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1115,7 +1115,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[41.4432403, 1.9817882999999998]</t>
+          <t>41.4432403,1.9817882999999998</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[41.4434046, 1.9816094]</t>
+          <t>41.4434046,1.9816094</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[41.4435864, 1.981409]</t>
+          <t>41.4435864,1.981409</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[41.4435987, 1.9813953]</t>
+          <t>41.4435987,1.9813953</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[41.4434627, 1.9815466]</t>
+          <t>41.4434627,1.9815466</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[41.4431857, 1.9818482000000002]</t>
+          <t>41.4431857,1.9818482000000002</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[41.4429595, 1.98211]</t>
+          <t>41.4429595,1.98211</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[41.430915899999995, 1.9947864000000002]</t>
+          <t>41.430915899999995,1.9947864000000002</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[41.4307456, 1.9948534]</t>
+          <t>41.4307456,1.9948534</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[41.4305783, 1.9949231]</t>
+          <t>41.4305783,1.9949231</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[41.4302531, 1.9950515]</t>
+          <t>41.4302531,1.9950515</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[41.4299349, 1.9951657]</t>
+          <t>41.4299349,1.9951657</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[41.4297779, 1.9952134]</t>
+          <t>41.4297779,1.9952134</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[41.4294856, 1.9952912]</t>
+          <t>41.4294856,1.9952912</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[41.4293491, 1.9953227]</t>
+          <t>41.4293491,1.9953227</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[41.4290997, 1.9953788000000001]</t>
+          <t>41.4290997,1.9953788000000001</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[41.428984, 1.9954051000000002]</t>
+          <t>41.428984,1.9954051000000002</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[41.4203103, 2.0008763]</t>
+          <t>41.4203103,2.0008763</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[41.4202427, 2.0009014]</t>
+          <t>41.4202427,2.0009014</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[41.4201112, 2.0009498]</t>
+          <t>41.4201112,2.0009498</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[41.4199846, 2.000996]</t>
+          <t>41.4199846,2.000996</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[41.4199223, 2.0010187]</t>
+          <t>41.4199223,2.0010187</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[41.419862, 2.0010391]</t>
+          <t>41.419862,2.0010391</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[41.4198032, 2.0010574]</t>
+          <t>41.4198032,2.0010574</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[41.419710099999996, 2.0010895]</t>
+          <t>41.419710099999996,2.0010895</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[41.41963, 2.0011187]</t>
+          <t>41.41963,2.0011187</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[41.419584900000004, 2.0011351]</t>
+          <t>41.419584900000004,2.0011351</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[41.4195708, 2.0012701]</t>
+          <t>41.4195708,2.0012701</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[41.419659700000004, 2.0011079]</t>
+          <t>41.419659700000004,2.0011079</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[41.4197117, 2.001089]</t>
+          <t>41.4197117,2.001089</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[41.419811800000005, 2.0010547]</t>
+          <t>41.419811800000005,2.0010547</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[41.4198531, 2.0010418]</t>
+          <t>41.4198531,2.0010418</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[41.4195717, 2.0011397]</t>
+          <t>41.4195717,2.0011397</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[41.419519, 2.0013575]</t>
+          <t>41.419519,2.0013575</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[41.4195388, 2.0014368]</t>
+          <t>41.4195388,2.0014368</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[41.4195733, 2.0016355]</t>
+          <t>41.4195733,2.0016355</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[41.4195923, 2.0017448]</t>
+          <t>41.4195923,2.0017448</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[41.4196118, 2.0018629]</t>
+          <t>41.4196118,2.0018629</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[41.419631800000005, 2.001989]</t>
+          <t>41.419631800000005,2.001989</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[41.4196503, 2.0021081]</t>
+          <t>41.4196503,2.0021081</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1995,7 +1995,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[41.4142114, 2.1317688]</t>
+          <t>41.4142114,2.1317688</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[41.424784, 2.1424843]</t>
+          <t>41.424784,2.1424843</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[41.4698098, 1.9225079999999999]</t>
+          <t>41.4698098,1.9225079999999999</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[41.3321438, 1.7107848]</t>
+          <t>41.3321438,1.7107848</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[41.3320834, 1.7108975]</t>
+          <t>41.3320834,1.7108975</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[41.3320202, 1.7110028]</t>
+          <t>41.3320202,1.7110028</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[41.3319076, 1.7111949]</t>
+          <t>41.3319076,1.7111949</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[41.331860299999995, 1.7112808]</t>
+          <t>41.331860299999995,1.7112808</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[41.3318196, 1.7113559]</t>
+          <t>41.3318196,1.7113559</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -2195,7 +2195,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[41.3313409, 1.7120085999999999]</t>
+          <t>41.3313409,1.7120085999999999</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[41.3311863, 1.7121885000000001]</t>
+          <t>41.3311863,1.7121885000000001</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -2239,7 +2239,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[41.331101600000004, 1.7122832000000001]</t>
+          <t>41.331101600000004,1.7122832000000001</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[41.316491, 1.7244887]</t>
+          <t>41.316491,1.7244887</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[41.3301193, 1.713328]</t>
+          <t>41.3301193,1.713328</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[41.3302302, 1.7132345999999998]</t>
+          <t>41.3302302,1.7132345999999998</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[41.3303381, 1.7131329000000002]</t>
+          <t>41.3303381,1.7131329000000002</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[41.330537799999995, 1.7129076]</t>
+          <t>41.330537799999995,1.7129076</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -2373,7 +2373,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[41.3307411, 1.7126847]</t>
+          <t>41.3307411,1.7126847</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[41.3308359, 1.7125815]</t>
+          <t>41.3308359,1.7125815</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[41.330923500000004, 1.7124854999999999]</t>
+          <t>41.330923500000004,1.7124854999999999</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[41.3310017, 1.7123957]</t>
+          <t>41.3310017,1.7123957</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[41.331133, 1.7122481]</t>
+          <t>41.331133,1.7122481</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[41.3311857, 1.7121892]</t>
+          <t>41.3311857,1.7121892</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[41.3312337, 1.7121332999999999]</t>
+          <t>41.3312337,1.7121332999999999</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[41.3313206, 1.7120322000000001]</t>
+          <t>41.3313206,1.7120322000000001</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[41.3313578, 1.7119888]</t>
+          <t>41.3313578,1.7119888</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[41.3318334, 1.7113304]</t>
+          <t>41.3318334,1.7113304</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[41.3319007, 1.7112073]</t>
+          <t>41.3319007,1.7112073</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[41.3319374, 1.7111414]</t>
+          <t>41.3319374,1.7111414</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[41.3319764, 1.7110738]</t>
+          <t>41.3319764,1.7110738</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2659,7 +2659,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[41.3320614, 1.710936]</t>
+          <t>41.3320614,1.710936</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>[41.332104, 1.7108591]</t>
+          <t>41.332104,1.7108591</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>[41.3322052, 1.7106729999999999]</t>
+          <t>41.3322052,1.7106729999999999</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>[41.334832999999996, 1.7043902]</t>
+          <t>41.334832999999996,1.7043902</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>[41.334775, 1.7042646]</t>
+          <t>41.334775,1.7042646</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>[41.3346733, 1.7040270000000002]</t>
+          <t>41.3346733,1.7040270000000002</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>[41.334622599999996, 1.7039019]</t>
+          <t>41.334622599999996,1.7039019</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>[41.3345105, 1.7036208]</t>
+          <t>41.3345105,1.7036208</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>[41.3344531, 1.7034585999999998]</t>
+          <t>41.3344531,1.7034585999999998</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>[41.3343967, 1.7032861]</t>
+          <t>41.3343967,1.7032861</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>[41.3343466, 1.7031098]</t>
+          <t>41.3343466,1.7031098</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>[41.3342504, 1.7027387]</t>
+          <t>41.3342504,1.7027387</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>[41.3342097, 1.7025457999999998]</t>
+          <t>41.3342097,1.7025457999999998</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>[41.3341689, 1.7023372]</t>
+          <t>41.3341689,1.7023372</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>[41.3341298, 1.7021176999999998]</t>
+          <t>41.3341298,1.7021176999999998</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>[41.334066, 1.7016365]</t>
+          <t>41.334066,1.7016365</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>[41.3325355, 1.6809007999999999]</t>
+          <t>41.3325355,1.6809007999999999</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>[41.332491499999996, 1.6808398]</t>
+          <t>41.332491499999996,1.6808398</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -3055,7 +3055,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>[41.3324537, 1.6807845000000001]</t>
+          <t>41.3324537,1.6807845000000001</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>[41.331623, 1.6794954]</t>
+          <t>41.331623,1.6794954</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -3099,7 +3099,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>[41.3314084, 1.67915]</t>
+          <t>41.3314084,1.67915</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>[41.3300987, 1.6772517999999998]</t>
+          <t>41.3300987,1.6772517999999998</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>[41.3300438, 1.6771826]</t>
+          <t>41.3300438,1.6771826</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>[41.3299458, 1.6770597]</t>
+          <t>41.3299458,1.6770597</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -3187,7 +3187,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>[41.3298596, 1.6769549]</t>
+          <t>41.3298596,1.6769549</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>[41.283710299999996, 1.4963695000000001]</t>
+          <t>41.283710299999996,1.4963695000000001</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -3231,7 +3231,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>[41.2799738, 1.4985553]</t>
+          <t>41.2799738,1.4985553</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>[41.279776, 1.4987106]</t>
+          <t>41.279776,1.4987106</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -3275,7 +3275,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>[41.279623900000004, 1.4988294]</t>
+          <t>41.279623900000004,1.4988294</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>[41.2795581, 1.4988825]</t>
+          <t>41.2795581,1.4988825</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>[41.279503399999996, 1.4989270000000001]</t>
+          <t>41.279503399999996,1.4989270000000001</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>[41.2794529, 1.4989693]</t>
+          <t>41.2794529,1.4989693</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>[41.2792819, 1.4991114]</t>
+          <t>41.2792819,1.4991114</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>[41.2792548, 1.4991338]</t>
+          <t>41.2792548,1.4991338</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -3407,7 +3407,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>[41.2792179, 1.4991641]</t>
+          <t>41.2792179,1.4991641</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>[41.2793581, 1.4990487]</t>
+          <t>41.2793581,1.4990487</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>[41.2794378, 1.4989819]</t>
+          <t>41.2794378,1.4989819</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>[41.2798155, 1.4986792999999998]</t>
+          <t>41.2798155,1.4986792999999998</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -3495,7 +3495,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[41.2799199, 1.4985972]</t>
+          <t>41.2799199,1.4985972</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>[41.2904222, 2.0108422]</t>
+          <t>41.2904222,2.0108422</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>[41.289085299999996, 2.0089796]</t>
+          <t>41.289085299999996,2.0089796</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>[41.2890466, 2.0087382000000003]</t>
+          <t>41.2890466,2.0087382000000003</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>[41.2890304, 2.008634]</t>
+          <t>41.2890304,2.008634</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -3605,7 +3605,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>[41.2970638, 1.9982855]</t>
+          <t>41.2970638,1.9982855</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -3627,7 +3627,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>[41.2972471, 1.9981157]</t>
+          <t>41.2972471,1.9981157</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>[41.297336200000004, 1.9980376000000002]</t>
+          <t>41.297336200000004,1.9980376000000002</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>[41.2975243, 1.9978870000000002]</t>
+          <t>41.2975243,1.9978870000000002</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -3693,7 +3693,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>[41.297623, 1.9978188000000001]</t>
+          <t>41.297623,1.9978188000000001</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>[41.2978067, 1.9977059]</t>
+          <t>41.2978067,1.9977059</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>[41.297891299999996, 1.9976585999999998]</t>
+          <t>41.297891299999996,1.9976585999999998</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>[41.2980309, 1.9975834]</t>
+          <t>41.2980309,1.9975834</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>[41.2980963, 1.997551]</t>
+          <t>41.2980963,1.997551</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>[41.2981568, 1.9975258999999999]</t>
+          <t>41.2981568,1.9975258999999999</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>[41.298271, 1.9974820999999998]</t>
+          <t>41.298271,1.9974820999999998</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>[41.299157799999996, 2.0011152]</t>
+          <t>41.299157799999996,2.0011152</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[41.2991089, 2.0012827]</t>
+          <t>41.2991089,2.0012827</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>[41.2990626, 2.0014579]</t>
+          <t>41.2990626,2.0014579</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>[41.29344, 2.007904]</t>
+          <t>41.29344,2.007904</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[41.2933079, 2.0080292]</t>
+          <t>41.2933079,2.0080292</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -3957,7 +3957,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[41.293050099999995, 2.0082753]</t>
+          <t>41.293050099999995,2.0082753</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[41.2927995, 2.0085154000000003]</t>
+          <t>41.2927995,2.0085154000000003</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[41.2926725, 2.0086404]</t>
+          <t>41.2926725,2.0086404</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[41.2924313, 2.0088977]</t>
+          <t>41.2924313,2.0088977</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[41.2922056, 2.0091303]</t>
+          <t>41.2922056,2.0091303</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -4067,7 +4067,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[41.2920962, 2.0092433]</t>
+          <t>41.2920962,2.0092433</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[41.291890699999996, 2.0094675]</t>
+          <t>41.291890699999996,2.0094675</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -4111,7 +4111,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[41.291786200000004, 2.0095682]</t>
+          <t>41.291786200000004,2.0095682</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[41.2916833, 2.0096689000000003]</t>
+          <t>41.2916833,2.0096689000000003</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -4155,7 +4155,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[41.29149, 2.0098566]</t>
+          <t>41.29149,2.0098566</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>[41.380668199999995, 2.1020967]</t>
+          <t>41.380668199999995,2.1020967</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>[41.3814446, 2.1023409]</t>
+          <t>41.3814446,2.1023409</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>[41.382158, 2.1038369]</t>
+          <t>41.382158,2.1038369</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>

</xml_diff>